<commit_message>
hypo reduction anova update
</commit_message>
<xml_diff>
--- a/knn_results/hypo_reduction.xlsx
+++ b/knn_results/hypo_reduction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tair\PycharmProjects\MAI-IML-W3\knn_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4D0647AF-5A8D-4AB6-80E1-CD991448EDDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D6759850-A870-4826-8F88-B42F4920CA71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -24,32 +24,16 @@
     <definedName name="_xlchart.v1.13" hidden="1">'10Folds'!$C$20:$C$29</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">'10Folds'!$D$19</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">'10Folds'!$D$20:$D$29</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'10Folds'!$A$19</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'10Folds'!$A$20:$A$29</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'10Folds'!$B$19</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'10Folds'!$B$20:$B$29</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'10Folds'!$A$2</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'10Folds'!$A$3:$A$12</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'10Folds'!$B$2</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'10Folds'!$B$3:$B$12</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'10Folds'!$B$2</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'10Folds'!$C$19</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'10Folds'!$C$20:$C$29</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'10Folds'!$D$19</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'10Folds'!$D$20:$D$29</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'10Folds'!$A$19</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'10Folds'!$A$20:$A$29</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'10Folds'!$B$19</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'10Folds'!$B$20:$B$29</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'10Folds'!$C$19</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'10Folds'!$C$20:$C$29</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'10Folds'!$C$2</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'10Folds'!$C$3:$C$12</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'10Folds'!$D$2</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'10Folds'!$D$3:$D$12</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'10Folds'!$B$3:$B$12</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'10Folds'!$D$19</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'10Folds'!$D$20:$D$29</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'10Folds'!$A$19</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'10Folds'!$A$20:$A$29</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'10Folds'!$B$19</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'10Folds'!$B$20:$B$29</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'10Folds'!$C$19</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'10Folds'!$C$20:$C$29</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'10Folds'!$D$19</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'10Folds'!$D$20:$D$29</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'10Folds'!$C$2</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'10Folds'!$C$3:$C$12</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'10Folds'!$D$2</definedName>
@@ -2547,19 +2531,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M37" sqref="M36:M37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2570,7 +2555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.99197860962566797</v>
       </c>
@@ -2601,7 +2586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.99465240641711195</v>
       </c>
@@ -2630,7 +2615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.99465240641711195</v>
       </c>
@@ -2647,19 +2632,19 @@
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="3">
-        <v>8.9304812834224574</v>
+        <v>9.9278074866310142</v>
       </c>
       <c r="J5" s="3">
-        <v>0.99227569815805083</v>
+        <v>0.9927807486631014</v>
       </c>
       <c r="K5" s="3">
-        <v>5.7987868620143219E-5</v>
+        <v>5.4095532233311781E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.97593582887700503</v>
       </c>
@@ -2676,19 +2661,19 @@
         <v>1</v>
       </c>
       <c r="H6" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" s="3">
-        <v>8.7780748663101562</v>
+        <v>9.7566844919786053</v>
       </c>
       <c r="J6" s="3">
-        <v>0.97534165181223953</v>
+        <v>0.97566844919786055</v>
       </c>
       <c r="K6" s="3">
-        <v>1.2113904061057432E-4</v>
+        <v>1.0874711252188624E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2705,19 +2690,19 @@
         <v>2</v>
       </c>
       <c r="H7" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I7" s="3">
-        <v>8.8903743315508006</v>
+        <v>9.8850267379679124</v>
       </c>
       <c r="J7" s="3">
-        <v>0.98781937017231114</v>
+        <v>0.98850267379679124</v>
       </c>
       <c r="K7" s="3">
-        <v>6.0966697487615508E-5</v>
+        <v>5.8861658421267782E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.99732620320855603</v>
       </c>
@@ -2734,19 +2719,19 @@
         <v>3</v>
       </c>
       <c r="H8" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I8" s="4">
-        <v>8.3716577540106929</v>
+        <v>9.2967914438502657</v>
       </c>
       <c r="J8" s="4">
-        <v>0.93018419489007698</v>
+        <v>0.92967914438502652</v>
       </c>
       <c r="K8" s="4">
-        <v>7.9435436465936646E-6</v>
+        <v>9.6116878123786721E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.99732620320855603</v>
       </c>
@@ -2760,7 +2745,7 @@
         <v>0.92780748663101598</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.98395721925133695</v>
       </c>
@@ -2774,7 +2759,7 @@
         <v>0.93315508021390303</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.99465240641711195</v>
       </c>
@@ -2791,7 +2776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.99732620320855603</v>
       </c>
@@ -2826,47 +2811,47 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="3">
-        <v>2.1777026318548803E-2</v>
+        <v>2.5082215676742244E-2</v>
       </c>
       <c r="I13" s="3">
         <v>3</v>
       </c>
       <c r="J13" s="3">
-        <v>7.2590087728496011E-3</v>
+        <v>8.3607385589140812E-3</v>
       </c>
       <c r="K13" s="3">
-        <v>117.06325060048019</v>
+        <v>144.57692307692278</v>
       </c>
       <c r="L13" s="3">
-        <v>2.4802046438958086E-17</v>
+        <v>3.9153362257028672E-20</v>
       </c>
       <c r="M13" s="3">
-        <v>2.9011195838408388</v>
+        <v>2.8662655509401795</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="G14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="3">
-        <v>1.9842972029194138E-3</v>
+        <v>2.0818439188996E-3</v>
       </c>
       <c r="I14" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J14" s="3">
-        <v>6.2009287591231681E-5</v>
+        <v>5.7828997747211107E-5</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2875,20 +2860,27 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="4">
-        <v>2.3761323521468217E-2</v>
+        <v>2.7164059595641842E-2</v>
       </c>
       <c r="I16" s="4">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3220,8 +3212,8 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A18:D18"/>
   </mergeCells>
-  <conditionalFormatting sqref="H2:M16">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="H2:M4 H9:M12 L5:M8">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3233,7 +3225,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:M31">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:M16">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>